<commit_message>
Fixed VINRefreshNoMatchOnRenewalAutoCA test for Auto Select, additional changes to UpdatedVIN tests
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/NoMatchORenewal_CA_SELECT.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/NoMatchORenewal_CA_SELECT.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gw3eraj\projects\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Reps\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -561,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AG7" sqref="AG7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -893,7 +893,7 @@
         <v>52</v>
       </c>
       <c r="AG3" s="2">
-        <v>20190612</v>
+        <v>20180612</v>
       </c>
       <c r="AH3" s="2" t="s">
         <v>29</v>

</xml_diff>